<commit_message>
Refactor js. Update data.
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\key\Web\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BBFF5F-B002-442E-BF2D-8566BA0EDA80}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1A002C-7116-4CA3-8379-397CFFCF7B22}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C011205-1D96-4F59-86A9-A33307C32E64}"/>
   </bookViews>
@@ -383,64 +383,64 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>-3.4184489395273001</c:v>
+                  <c:v>-3.3880685093911098</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.11012907315386</c:v>
+                  <c:v>-3.0806869660071499</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.8018092067804199</c:v>
+                  <c:v>-2.7733054226231899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.4934893404069798</c:v>
+                  <c:v>-2.46592387923923</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.1851694740335401</c:v>
+                  <c:v>-2.1585423358552802</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.8768496076601</c:v>
+                  <c:v>-1.85116079247132</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.5685297412866599</c:v>
+                  <c:v>-1.5437792490873601</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.26020987491322</c:v>
+                  <c:v>-1.2363977057033999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.951890008539785</c:v>
+                  <c:v>-0.92901616231944595</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.643570142166346</c:v>
+                  <c:v>-0.62163461893548899</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.335250275792907</c:v>
+                  <c:v>-0.31425307555153098</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-2.6930409419468001E-2</c:v>
+                  <c:v>-6.8715321675740801E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.281389456953971</c:v>
+                  <c:v>0.30051001121638299</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.58970932332741</c:v>
+                  <c:v>0.60789155460034106</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.898029189700849</c:v>
+                  <c:v>0.91527309798429801</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.20634905607429</c:v>
+                  <c:v>1.22265464136826</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5146689224477301</c:v>
+                  <c:v>1.5300361847522099</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.82298878882117</c:v>
+                  <c:v>1.8374177281361701</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.1313086551946099</c:v>
+                  <c:v>2.1447992715201298</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.4396285215680402</c:v>
+                  <c:v>2.4521808149040898</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -452,64 +452,64 @@
                 <c:formatCode>_-* #\ ##0_-;\-* #\ ##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>772</c:v>
+                  <c:v>838</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4667</c:v>
+                  <c:v>5024</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11506</c:v>
+                  <c:v>11580</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23540</c:v>
+                  <c:v>23766</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42749</c:v>
+                  <c:v>44450</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50747</c:v>
+                  <c:v>52212</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>55952</c:v>
+                  <c:v>56276</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>61355</c:v>
+                  <c:v>61278</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>65449</c:v>
+                  <c:v>67183</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>63870</c:v>
+                  <c:v>62896</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>54385</c:v>
+                  <c:v>52902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51476</c:v>
+                  <c:v>52667</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>50511</c:v>
+                  <c:v>51614</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36790</c:v>
+                  <c:v>35512</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26199</c:v>
+                  <c:v>25722</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16895</c:v>
+                  <c:v>16699</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4868</c:v>
+                  <c:v>4677</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>633</c:v>
+                  <c:v>561</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1689,7 +1689,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1EE58F1-E347-444C-A3E6-43601D66C21E}">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:N23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1739,10 +1741,10 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="4">
-        <v>-3.4184489395273001</v>
+        <v>-3.3880685093911098</v>
       </c>
       <c r="C3" s="8">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1760,10 +1762,10 @@
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="5">
-        <v>-3.11012907315386</v>
+        <v>-3.0806869660071499</v>
       </c>
       <c r="C4" s="9">
-        <v>772</v>
+        <v>838</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1781,10 +1783,10 @@
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="5">
-        <v>-2.8018092067804199</v>
+        <v>-2.7733054226231899</v>
       </c>
       <c r="C5" s="9">
-        <v>4667</v>
+        <v>5024</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1802,10 +1804,10 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="5">
-        <v>-2.4934893404069798</v>
+        <v>-2.46592387923923</v>
       </c>
       <c r="C6" s="9">
-        <v>11506</v>
+        <v>11580</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1823,10 +1825,10 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="5">
-        <v>-2.1851694740335401</v>
+        <v>-2.1585423358552802</v>
       </c>
       <c r="C7" s="9">
-        <v>23540</v>
+        <v>23766</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1844,10 +1846,10 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="5">
-        <v>-1.8768496076601</v>
+        <v>-1.85116079247132</v>
       </c>
       <c r="C8" s="9">
-        <v>42749</v>
+        <v>44450</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1865,10 +1867,10 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="5">
-        <v>-1.5685297412866599</v>
+        <v>-1.5437792490873601</v>
       </c>
       <c r="C9" s="9">
-        <v>50747</v>
+        <v>52212</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1886,10 +1888,10 @@
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="5">
-        <v>-1.26020987491322</v>
+        <v>-1.2363977057033999</v>
       </c>
       <c r="C10" s="9">
-        <v>55952</v>
+        <v>56276</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1907,10 +1909,10 @@
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="5">
-        <v>-0.951890008539785</v>
+        <v>-0.92901616231944595</v>
       </c>
       <c r="C11" s="9">
-        <v>61355</v>
+        <v>61278</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1928,10 +1930,10 @@
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="5">
-        <v>-0.643570142166346</v>
+        <v>-0.62163461893548899</v>
       </c>
       <c r="C12" s="9">
-        <v>65449</v>
+        <v>67183</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1949,10 +1951,10 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="5">
-        <v>-0.335250275792907</v>
+        <v>-0.31425307555153098</v>
       </c>
       <c r="C13" s="9">
-        <v>63870</v>
+        <v>62896</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1970,10 +1972,10 @@
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="5">
-        <v>-2.6930409419468001E-2</v>
+        <v>-6.8715321675740801E-3</v>
       </c>
       <c r="C14" s="9">
-        <v>54385</v>
+        <v>52902</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1991,10 +1993,10 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="5">
-        <v>0.281389456953971</v>
+        <v>0.30051001121638299</v>
       </c>
       <c r="C15" s="9">
-        <v>51476</v>
+        <v>52667</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2012,10 +2014,10 @@
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="5">
-        <v>0.58970932332741</v>
+        <v>0.60789155460034106</v>
       </c>
       <c r="C16" s="9">
-        <v>50511</v>
+        <v>51614</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2033,10 +2035,10 @@
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="5">
-        <v>0.898029189700849</v>
+        <v>0.91527309798429801</v>
       </c>
       <c r="C17" s="9">
-        <v>36790</v>
+        <v>35512</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2054,10 +2056,10 @@
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="6">
-        <v>1.20634905607429</v>
+        <v>1.22265464136826</v>
       </c>
       <c r="C18" s="9">
-        <v>26199</v>
+        <v>25722</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2075,10 +2077,10 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="6">
-        <v>1.5146689224477301</v>
+        <v>1.5300361847522099</v>
       </c>
       <c r="C19" s="9">
-        <v>16895</v>
+        <v>16699</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -2096,10 +2098,10 @@
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="6">
-        <v>1.82298878882117</v>
+        <v>1.8374177281361701</v>
       </c>
       <c r="C20" s="9">
-        <v>4868</v>
+        <v>4677</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2117,10 +2119,10 @@
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="6">
-        <v>2.1313086551946099</v>
+        <v>2.1447992715201298</v>
       </c>
       <c r="C21" s="9">
-        <v>633</v>
+        <v>561</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2138,10 +2140,10 @@
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="7">
-        <v>2.4396285215680402</v>
+        <v>2.4521808149040898</v>
       </c>
       <c r="C22" s="10">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>

</xml_diff>